<commit_message>
this is my last opencart-testng
</commit_message>
<xml_diff>
--- a/Testdata/Copy of Opencart_LoginData.xlsx
+++ b/Testdata/Copy of Opencart_LoginData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dilip\Desktop\ALL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\eclipse\opencart\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E9FB8AD-6BCA-461A-BC06-2280DA50EACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E0A34B-5CEA-4399-96F0-EB95FD188CD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{1F2D179E-37D2-4BC0-88A9-F5C135B87DA5}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>username</t>
   </si>
@@ -67,9 +67,6 @@
   </si>
   <si>
     <t>result</t>
-  </si>
-  <si>
-    <t>dilipmohapatra2015@gmail.com</t>
   </si>
   <si>
     <t>valid</t>
@@ -494,7 +491,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -517,13 +514,13 @@
     </row>
     <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.5">
       <c r="A2" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.5">
@@ -561,13 +558,13 @@
     </row>
     <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.5">
       <c r="A6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="C6" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>